<commit_message>
Tuning hyperparameters Random forest
</commit_message>
<xml_diff>
--- a/Data/Hashtags.xlsx
+++ b/Data/Hashtags.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s157165\Documents\Jaar 5 2019-2020 Master\Internship Australia\InternshipOneOnEpsilon\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BD48F53-879D-46F7-A7E0-D1811C5EAD5A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F0A1EFE-A56C-4451-A164-DEB93E2EFBD7}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{03EEA932-B2E2-455D-8D16-46A831B31555}"/>
   </bookViews>
@@ -2346,8 +2346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0169DE-9321-4416-B3C2-4B60D6FCFF10}">
   <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B62" sqref="B62:B82"/>
+    <sheetView topLeftCell="G1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M1" sqref="M1:M1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4536,8 +4536,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95734453-97CD-4121-968D-832BD54966BB}">
   <dimension ref="A1:K109"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="D81" sqref="D81"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>